<commit_message>
Added Data Master form Futures
</commit_message>
<xml_diff>
--- a/Rest API/Script/ProductIdToPull.xlsx
+++ b/Rest API/Script/ProductIdToPull.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranlev\Documents\Horizon OMS UAT\Rest API\Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135F5ED9-CF3C-404D-BEC1-709BCD740299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D024073-5E48-4607-87A0-4124097EC848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="5910" windowWidth="14400" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,17 +363,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1003</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>